<commit_message>
Update action plan with next steps
</commit_message>
<xml_diff>
--- a/TeamPortfolio/ActionPlan.xlsx
+++ b/TeamPortfolio/ActionPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beckygriffiths/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beckygriffiths/Documents/Docs/University/Assignments/12.11_ComputationalSkillsCodingProject/HPDM172_assignment/TeamPortfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C1352F-8CBC-354E-85DA-4560C221AC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFFE3EC-11D7-E546-9CE0-40B22B1C2D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="7560" windowWidth="28160" windowHeight="15840" xr2:uid="{4014695D-D392-41D2-A24E-6252DB29BD94}"/>
+    <workbookView xWindow="1260" yWindow="3280" windowWidth="28140" windowHeight="15840" xr2:uid="{4014695D-D392-41D2-A24E-6252DB29BD94}"/>
   </bookViews>
   <sheets>
     <sheet name="Action Plan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Group</t>
   </si>
@@ -98,21 +98,12 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>&lt;insert task here&gt;</t>
-  </si>
-  <si>
     <t>GOAL #1 Create database</t>
   </si>
   <si>
     <t>Create ERD to describe relationships between tables</t>
   </si>
   <si>
-    <t>Generate data for input into database tables</t>
-  </si>
-  <si>
-    <t>Create database in MySQL</t>
-  </si>
-  <si>
     <t>GOAL #2 Create SQL queries</t>
   </si>
   <si>
@@ -122,7 +113,37 @@
     <t>BG</t>
   </si>
   <si>
-    <t>GOAL #3 Create documentation</t>
+    <t>Queries 1–5 + documentation</t>
+  </si>
+  <si>
+    <t>Queries 6–10 + documentation</t>
+  </si>
+  <si>
+    <t>Queries 11–15 + documentation</t>
+  </si>
+  <si>
+    <t>Queries 16–19 + documentation</t>
+  </si>
+  <si>
+    <t>GOAL #3 Polish documentation</t>
+  </si>
+  <si>
+    <t>Generate data for input into database tables + document process</t>
+  </si>
+  <si>
+    <t>Create database in MySQL + document process</t>
+  </si>
+  <si>
+    <t>Create github pages website</t>
+  </si>
+  <si>
+    <t>Finalise main README.md file</t>
+  </si>
+  <si>
+    <t>Finalise README.md file for sql_queries subdirectory</t>
+  </si>
+  <si>
+    <t>Finalise README.md file for data_generation subdirectory</t>
   </si>
 </sst>
 </file>
@@ -268,6 +289,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,7 +299,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D273DF14-D9EA-4740-83D2-767564C2185A}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,10 +664,10 @@
       <c r="C1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
@@ -661,12 +682,12 @@
       <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -678,15 +699,15 @@
       <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
@@ -712,22 +733,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="A7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -735,19 +756,19 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>45983</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <v>45995</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -755,19 +776,19 @@
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>45983</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>45995</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -775,46 +796,73 @@
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>45983</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>45995</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -834,13 +882,13 @@
           <x14:formula1>
             <xm:f>Settings!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C8:C10 C13:C15 C17:C18</xm:sqref>
+          <xm:sqref>C8:C10 C13:C15 C20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C370556-BAB4-4BEC-B4D1-C0B88505EA19}">
           <x14:formula1>
             <xm:f>Settings!$B$3:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D8:D10 D13:D15 D17:D18</xm:sqref>
+          <xm:sqref>D8:D10 D13:D15 D19:D20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Make sure all fields are filled out in action plan
</commit_message>
<xml_diff>
--- a/TeamPortfolio/ActionPlan.xlsx
+++ b/TeamPortfolio/ActionPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beckygriffiths/Documents/Docs/University/Assignments/12.11_ComputationalSkillsCodingProject/HPDM172_assignment/TeamPortfolio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beckygriffiths/Documents/Docs/University/Assignments/12.11_ComputationalSkillsCodingProject/690052013_700079488_750012749_750069207_HPDM172_group_coding_assignment_2025-26/HPDM172_assignment/TeamPortfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8951F3DC-383D-484D-AE55-40B19A4D46A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D29B4E-9769-6048-9B7A-47483632BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15320" yWindow="680" windowWidth="14080" windowHeight="18440" xr2:uid="{4014695D-D392-41D2-A24E-6252DB29BD94}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>ACTION PLAN</t>
   </si>
   <si>
@@ -56,15 +53,9 @@
     <t>ACTION</t>
   </si>
   <si>
-    <t>Project Summary</t>
-  </si>
-  <si>
     <t>PRIORITY</t>
   </si>
   <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>START DATE</t>
   </si>
   <si>
@@ -156,6 +147,15 @@
   </si>
   <si>
     <t>Make README.md file for sql_queries subdirectory</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>Project Name: HPDM172 Group Coding Assignment</t>
+  </si>
+  <si>
+    <t>Project Summary: Developing a synthetic health data science database in MySQL</t>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D273DF14-D9EA-4740-83D2-767564C2185A}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D25"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,11 +670,11 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="12" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -692,7 +692,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -712,7 +712,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -723,30 +723,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>2</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -757,16 +757,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" s="14">
         <v>45983</v>
@@ -777,16 +777,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E9" s="14">
         <v>45983</v>
@@ -797,16 +797,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E10" s="14">
         <v>45983</v>
@@ -817,16 +817,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E11" s="14">
         <v>45996</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -848,16 +848,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E15" s="14">
         <v>45985</v>
@@ -868,16 +868,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E16" s="14">
         <v>45985</v>
@@ -888,16 +888,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E17" s="14">
         <v>45985</v>
@@ -908,16 +908,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E18" s="14">
         <v>45985</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -945,16 +945,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E22" s="14">
         <v>45985</v>
@@ -965,16 +965,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E23" s="14">
         <v>45985</v>
@@ -985,16 +985,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E24" s="14">
         <v>45985</v>
@@ -1005,16 +1005,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E25" s="14">
         <v>45985</v>
@@ -1069,39 +1069,39 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>